<commit_message>
Code changes for THS template E!
</commit_message>
<xml_diff>
--- a/MasterData/1. AmortTemplateUSA Network.xlsx
+++ b/MasterData/1. AmortTemplateUSA Network.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mohammed.saquib\eclipse-workspace\amorttemplate\MasterData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\206534643\git\AmortTemplateAutomation\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
@@ -742,12 +742,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="434791480"/>
-        <c:axId val="434793048"/>
+        <c:axId val="221966312"/>
+        <c:axId val="221965528"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:valAx>
-        <c:axId val="434793048"/>
+        <c:axId val="221965528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,12 +798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434791480"/>
+        <c:crossAx val="221966312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="434791480"/>
+        <c:axId val="221966312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434793048"/>
+        <c:crossAx val="221965528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4339,8 +4339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView topLeftCell="D97" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N127"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9665,7 +9665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Code added for generating merged report for all networks
</commit_message>
<xml_diff>
--- a/MasterData/1. AmortTemplateUSA Network.xlsx
+++ b/MasterData/1. AmortTemplateUSA Network.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\206534643\git\AmortTemplateAutomation\MasterData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mohammed.saquib\eclipse-workspace\amorttemplate\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
-    <sheet name="AmortTemplateGrid-Reason" sheetId="2" r:id="rId2"/>
+    <sheet name="AmortTemplateGrid" sheetId="2" r:id="rId2"/>
     <sheet name="AmortTemplateSectionGrid" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'AmortTemplateGrid-Reason'!$A$1:$N$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">AmortTemplateGrid!$A$1:$N$127</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AmortTemplateSectionGrid!$A$1:$F$235</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -742,12 +742,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="221966312"/>
-        <c:axId val="221965528"/>
+        <c:axId val="370057864"/>
+        <c:axId val="370364520"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:valAx>
-        <c:axId val="221965528"/>
+        <c:axId val="370364520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,12 +798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221966312"/>
+        <c:crossAx val="370057864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="221966312"/>
+        <c:axId val="370057864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221965528"/>
+        <c:crossAx val="370364520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1521,7 +1521,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mohammed Saquib" refreshedDate="43215.677294444446" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="126">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:N127" sheet="AmortTemplateGrid-Reason"/>
+    <worksheetSource ref="A1:N127" sheet="AmortTemplateGrid"/>
   </cacheSource>
   <cacheFields count="14">
     <cacheField name="AmortTemplateNo" numFmtId="0">
@@ -4337,11 +4337,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N133"/>
+  <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9646,11 +9644,6 @@
       <c r="M127" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates test results for all Networks
</commit_message>
<xml_diff>
--- a/MasterData/1. AmortTemplateUSA Network.xlsx
+++ b/MasterData/1. AmortTemplateUSA Network.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mohammed.saquib\eclipse-workspace\amorttemplate\MasterData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\206534643\git\AmortTemplateAutomation\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
@@ -742,12 +742,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="370057864"/>
-        <c:axId val="370364520"/>
+        <c:axId val="214927696"/>
+        <c:axId val="214929264"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:valAx>
-        <c:axId val="370364520"/>
+        <c:axId val="214929264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,12 +798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="370057864"/>
+        <c:crossAx val="214927696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="370057864"/>
+        <c:axId val="214927696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="370364520"/>
+        <c:crossAx val="214929264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>

</xml_diff>